<commit_message>
update tabel Kelas and Mahasiswa logic for excel import
</commit_message>
<xml_diff>
--- a/public/template_kelas_sikurft.xlsx
+++ b/public/template_kelas_sikurft.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GHANI\Semester 5\PKL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\SI-KurFT\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC32CF83-3F25-48CE-9798-A0AA94093C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6999079-5941-4044-A989-B68E753DD8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>nama</t>
-  </si>
-  <si>
-    <t>nim</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>NIM</t>
+  </si>
+  <si>
+    <t>NAMA</t>
+  </si>
+  <si>
+    <t>FAKULTAS</t>
+  </si>
+  <si>
+    <t>PROGRAM STUDI</t>
+  </si>
+  <si>
+    <t>ANGKATAN</t>
+  </si>
+  <si>
+    <t>JENIS KELAMIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +57,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,13 +86,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,27 +395,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New some seeder file
</commit_message>
<xml_diff>
--- a/public/template_kelas_sikurft.xlsx
+++ b/public/template_kelas_sikurft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\SI-KurFT\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6999079-5941-4044-A989-B68E753DD8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9671D7E-6085-4EAB-95C8-AD6EE8FD8293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="750" windowWidth="28785" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NIM</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>JENIS KELAMIN</t>
+  </si>
+  <si>
+    <t>STATUS</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,10 +411,10 @@
     <col min="3" max="3" width="25.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="35.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="26.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -429,6 +432,9 @@
       </c>
       <c r="F1" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>